<commit_message>
heh sums, wes bengi
</commit_message>
<xml_diff>
--- a/excel/import penawaran.xlsx
+++ b/excel/import penawaran.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/fa_sai/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8D45F8-AFC8-A942-B5B6-97C274CD4AF8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A378BC8-A935-6A44-84A9-261DD5ECFBB2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" xr2:uid="{B264C883-C65C-404D-AD50-16A2D4E1BD84}"/>
   </bookViews>
@@ -531,9 +531,6 @@
     <t>190</t>
   </si>
   <si>
-    <t>0.23364</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
@@ -979,6 +976,9 @@
   </si>
   <si>
     <t>HZY</t>
+  </si>
+  <si>
+    <t>0.2397</t>
   </si>
 </sst>
 </file>
@@ -1498,8 +1498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4D0551A-2F20-8F4C-8743-DC3D731B472A}">
   <dimension ref="A1:AC68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C35" workbookViewId="0">
-      <selection activeCell="W18" sqref="W18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3035,7 +3035,7 @@
         <v>120</v>
       </c>
       <c r="P20" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="Q20" s="6" t="s">
         <v>47</v>
@@ -3784,13 +3784,13 @@
         <v>167</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>168</v>
+        <v>317</v>
       </c>
       <c r="J30" s="6" t="s">
         <v>34</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>168</v>
+        <v>317</v>
       </c>
       <c r="L30" s="6" t="s">
         <v>34</v>
@@ -3814,7 +3814,7 @@
         <v>57</v>
       </c>
       <c r="S30" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T30" s="6"/>
       <c r="U30" s="6"/>
@@ -3849,16 +3849,16 @@
         <v>30</v>
       </c>
       <c r="E31" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="F31" s="6" t="s">
         <v>171</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>172</v>
       </c>
       <c r="G31" s="6" t="s">
         <v>33</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I31" s="6" t="s">
         <v>136</v>
@@ -3867,7 +3867,7 @@
         <v>34</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L31" s="6" t="s">
         <v>34</v>
@@ -3879,7 +3879,7 @@
         <v>110</v>
       </c>
       <c r="O31" s="6" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="P31" s="18" t="s">
         <v>112</v>
@@ -3891,7 +3891,7 @@
         <v>57</v>
       </c>
       <c r="S31" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T31" s="6"/>
       <c r="U31" s="6"/>
@@ -3926,16 +3926,16 @@
         <v>30</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>33</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I32" s="6" t="s">
         <v>140</v>
@@ -3944,7 +3944,7 @@
         <v>34</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L32" s="6" t="s">
         <v>34</v>
@@ -3956,7 +3956,7 @@
         <v>119</v>
       </c>
       <c r="O32" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="P32" s="19" t="s">
         <v>112</v>
@@ -3968,7 +3968,7 @@
         <v>57</v>
       </c>
       <c r="S32" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T32" s="6"/>
       <c r="U32" s="6"/>
@@ -4003,10 +4003,10 @@
         <v>30</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G33" s="6" t="s">
         <v>33</v>
@@ -4021,7 +4021,7 @@
         <v>34</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L33" s="6" t="s">
         <v>34</v>
@@ -4030,10 +4030,10 @@
         <v>46</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O33" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="P33" s="20" t="s">
         <v>112</v>
@@ -4045,7 +4045,7 @@
         <v>57</v>
       </c>
       <c r="S33" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T33" s="6"/>
       <c r="U33" s="6"/>
@@ -4063,7 +4063,7 @@
         <v>38</v>
       </c>
       <c r="AC33" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="34" spans="1:29">
@@ -4080,16 +4080,16 @@
         <v>30</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G34" s="6" t="s">
         <v>33</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I34" s="6" t="s">
         <v>145</v>
@@ -4098,7 +4098,7 @@
         <v>34</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L34" s="6" t="s">
         <v>34</v>
@@ -4107,13 +4107,13 @@
         <v>46</v>
       </c>
       <c r="N34" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O34" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="P34" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="Q34" s="6" t="s">
         <v>113</v>
@@ -4122,7 +4122,7 @@
         <v>57</v>
       </c>
       <c r="S34" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T34" s="6"/>
       <c r="U34" s="6"/>
@@ -4140,7 +4140,7 @@
         <v>38</v>
       </c>
       <c r="AC34" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="35" spans="1:29">
@@ -4157,10 +4157,10 @@
         <v>30</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G35" s="6" t="s">
         <v>33</v>
@@ -4175,7 +4175,7 @@
         <v>34</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L35" s="6" t="s">
         <v>34</v>
@@ -4187,7 +4187,7 @@
         <v>157</v>
       </c>
       <c r="O35" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="P35" s="18" t="s">
         <v>147</v>
@@ -4199,7 +4199,7 @@
         <v>57</v>
       </c>
       <c r="S35" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T35" s="6"/>
       <c r="U35" s="6"/>
@@ -4217,7 +4217,7 @@
         <v>38</v>
       </c>
       <c r="AC35" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="36" spans="1:29">
@@ -4234,10 +4234,10 @@
         <v>30</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>33</v>
@@ -4252,7 +4252,7 @@
         <v>34</v>
       </c>
       <c r="K36" s="6" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L36" s="6" t="s">
         <v>34</v>
@@ -4264,10 +4264,10 @@
         <v>157</v>
       </c>
       <c r="O36" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="P36" s="19" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="Q36" s="6" t="s">
         <v>113</v>
@@ -4276,7 +4276,7 @@
         <v>57</v>
       </c>
       <c r="S36" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T36" s="6"/>
       <c r="U36" s="6"/>
@@ -4294,7 +4294,7 @@
         <v>38</v>
       </c>
       <c r="AC36" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="37" spans="1:29">
@@ -4311,16 +4311,16 @@
         <v>30</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>33</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I37" s="6" t="s">
         <v>67</v>
@@ -4329,7 +4329,7 @@
         <v>34</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="L37" s="6" t="s">
         <v>34</v>
@@ -4338,13 +4338,13 @@
         <v>46</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O37" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="P37" s="18" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="Q37" s="6" t="s">
         <v>113</v>
@@ -4353,7 +4353,7 @@
         <v>57</v>
       </c>
       <c r="S37" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T37" s="6"/>
       <c r="U37" s="6"/>
@@ -4388,16 +4388,16 @@
         <v>30</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G38" s="6" t="s">
         <v>33</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I38" s="6" t="s">
         <v>72</v>
@@ -4406,7 +4406,7 @@
         <v>34</v>
       </c>
       <c r="K38" s="6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L38" s="6" t="s">
         <v>34</v>
@@ -4418,10 +4418,10 @@
         <v>157</v>
       </c>
       <c r="O38" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="P38" s="18" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="Q38" s="6" t="s">
         <v>113</v>
@@ -4430,7 +4430,7 @@
         <v>57</v>
       </c>
       <c r="S38" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T38" s="6"/>
       <c r="U38" s="6"/>
@@ -4465,16 +4465,16 @@
         <v>30</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G39" s="6" t="s">
         <v>33</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I39" s="6" t="s">
         <v>75</v>
@@ -4483,7 +4483,7 @@
         <v>34</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L39" s="6" t="s">
         <v>34</v>
@@ -4495,10 +4495,10 @@
         <v>157</v>
       </c>
       <c r="O39" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="P39" s="18" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Q39" s="6" t="s">
         <v>113</v>
@@ -4507,7 +4507,7 @@
         <v>57</v>
       </c>
       <c r="S39" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T39" s="6"/>
       <c r="U39" s="6"/>
@@ -4542,16 +4542,16 @@
         <v>30</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>33</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I40" s="6" t="s">
         <v>79</v>
@@ -4560,7 +4560,7 @@
         <v>34</v>
       </c>
       <c r="K40" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L40" s="6" t="s">
         <v>34</v>
@@ -4569,13 +4569,13 @@
         <v>46</v>
       </c>
       <c r="N40" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O40" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="P40" s="18" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Q40" s="6" t="s">
         <v>113</v>
@@ -4584,7 +4584,7 @@
         <v>57</v>
       </c>
       <c r="S40" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T40" s="6"/>
       <c r="U40" s="6"/>
@@ -4619,16 +4619,16 @@
         <v>30</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>33</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="I41" s="6" t="s">
         <v>67</v>
@@ -4637,7 +4637,7 @@
         <v>34</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L41" s="6" t="s">
         <v>34</v>
@@ -4649,10 +4649,10 @@
         <v>157</v>
       </c>
       <c r="O41" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="P41" s="21" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="Q41" s="6" t="s">
         <v>113</v>
@@ -4661,7 +4661,7 @@
         <v>57</v>
       </c>
       <c r="S41" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T41" s="6"/>
       <c r="U41" s="6"/>
@@ -4696,16 +4696,16 @@
         <v>30</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>33</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="I42" s="6" t="s">
         <v>84</v>
@@ -4714,7 +4714,7 @@
         <v>34</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L42" s="6" t="s">
         <v>34</v>
@@ -4726,10 +4726,10 @@
         <v>157</v>
       </c>
       <c r="O42" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P42" s="21" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="Q42" s="6" t="s">
         <v>113</v>
@@ -4738,7 +4738,7 @@
         <v>57</v>
       </c>
       <c r="S42" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T42" s="6"/>
       <c r="U42" s="6"/>
@@ -4773,16 +4773,16 @@
         <v>30</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G43" s="6" t="s">
         <v>33</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I43" s="6" t="s">
         <v>87</v>
@@ -4791,7 +4791,7 @@
         <v>34</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L43" s="6" t="s">
         <v>34</v>
@@ -4800,13 +4800,13 @@
         <v>46</v>
       </c>
       <c r="N43" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O43" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="P43" s="21" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="Q43" s="6" t="s">
         <v>113</v>
@@ -4815,7 +4815,7 @@
         <v>57</v>
       </c>
       <c r="S43" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T43" s="6"/>
       <c r="U43" s="6"/>
@@ -4850,16 +4850,16 @@
         <v>30</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G44" s="6" t="s">
         <v>33</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I44" s="6" t="s">
         <v>89</v>
@@ -4868,7 +4868,7 @@
         <v>34</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L44" s="6" t="s">
         <v>34</v>
@@ -4877,13 +4877,13 @@
         <v>46</v>
       </c>
       <c r="N44" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O44" s="6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="P44" s="18" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="Q44" s="6" t="s">
         <v>113</v>
@@ -4892,7 +4892,7 @@
         <v>57</v>
       </c>
       <c r="S44" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T44" s="6"/>
       <c r="U44" s="6"/>
@@ -4927,16 +4927,16 @@
         <v>30</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G45" s="6" t="s">
         <v>33</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="I45" s="6" t="s">
         <v>95</v>
@@ -4945,7 +4945,7 @@
         <v>34</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L45" s="6" t="s">
         <v>34</v>
@@ -4957,10 +4957,10 @@
         <v>157</v>
       </c>
       <c r="O45" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="P45" s="18" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="Q45" s="6" t="s">
         <v>113</v>
@@ -4969,7 +4969,7 @@
         <v>43</v>
       </c>
       <c r="S45" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T45" s="6"/>
       <c r="U45" s="6"/>
@@ -5004,16 +5004,16 @@
         <v>30</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G46" s="6" t="s">
         <v>33</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I46" s="6" t="s">
         <v>100</v>
@@ -5022,7 +5022,7 @@
         <v>34</v>
       </c>
       <c r="K46" s="6" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L46" s="6" t="s">
         <v>34</v>
@@ -5031,13 +5031,13 @@
         <v>46</v>
       </c>
       <c r="N46" s="6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O46" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="P46" s="22" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="Q46" s="6" t="s">
         <v>113</v>
@@ -5046,7 +5046,7 @@
         <v>43</v>
       </c>
       <c r="S46" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T46" s="6"/>
       <c r="U46" s="6"/>
@@ -5064,7 +5064,7 @@
         <v>38</v>
       </c>
       <c r="AC46" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="47" spans="1:29">
@@ -5081,16 +5081,16 @@
         <v>30</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G47" s="6" t="s">
         <v>33</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I47" s="6" t="s">
         <v>104</v>
@@ -5099,7 +5099,7 @@
         <v>34</v>
       </c>
       <c r="K47" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="L47" s="6" t="s">
         <v>34</v>
@@ -5108,10 +5108,10 @@
         <v>46</v>
       </c>
       <c r="N47" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="O47" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="P47" s="18" t="s">
         <v>51</v>
@@ -5123,7 +5123,7 @@
         <v>43</v>
       </c>
       <c r="S47" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T47" s="6"/>
       <c r="U47" s="6"/>
@@ -5141,7 +5141,7 @@
         <v>38</v>
       </c>
       <c r="AC47" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="48" spans="1:29">
@@ -5158,25 +5158,25 @@
         <v>30</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G48" s="6" t="s">
         <v>33</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J48" s="6" t="s">
         <v>34</v>
       </c>
       <c r="K48" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="L48" s="6" t="s">
         <v>34</v>
@@ -5185,13 +5185,13 @@
         <v>46</v>
       </c>
       <c r="N48" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="O48" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="P48" s="18" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="Q48" s="6" t="s">
         <v>113</v>
@@ -5200,7 +5200,7 @@
         <v>43</v>
       </c>
       <c r="S48" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T48" s="6"/>
       <c r="U48" s="6"/>
@@ -5218,7 +5218,7 @@
         <v>38</v>
       </c>
       <c r="AC48" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="49" spans="1:29">
@@ -5235,25 +5235,25 @@
         <v>30</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G49" s="6" t="s">
         <v>33</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I49" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J49" s="6" t="s">
         <v>34</v>
       </c>
       <c r="K49" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="L49" s="6" t="s">
         <v>34</v>
@@ -5262,10 +5262,10 @@
         <v>46</v>
       </c>
       <c r="N49" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="O49" s="6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="P49" s="18" t="s">
         <v>41</v>
@@ -5277,7 +5277,7 @@
         <v>57</v>
       </c>
       <c r="S49" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T49" s="6"/>
       <c r="U49" s="6"/>
@@ -5295,7 +5295,7 @@
         <v>38</v>
       </c>
       <c r="AC49" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="50" spans="1:29">
@@ -5312,25 +5312,25 @@
         <v>30</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G50" s="6" t="s">
         <v>33</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J50" s="6" t="s">
         <v>34</v>
       </c>
       <c r="K50" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L50" s="6" t="s">
         <v>34</v>
@@ -5339,10 +5339,10 @@
         <v>46</v>
       </c>
       <c r="N50" s="6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="O50" s="6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="P50" s="18" t="s">
         <v>121</v>
@@ -5354,7 +5354,7 @@
         <v>43</v>
       </c>
       <c r="S50" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T50" s="6"/>
       <c r="U50" s="6"/>
@@ -5372,7 +5372,7 @@
         <v>38</v>
       </c>
       <c r="AC50" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="51" spans="1:29">
@@ -5389,25 +5389,25 @@
         <v>30</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G51" s="6" t="s">
         <v>33</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J51" s="6" t="s">
         <v>34</v>
       </c>
       <c r="K51" s="6" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="L51" s="6" t="s">
         <v>34</v>
@@ -5416,13 +5416,13 @@
         <v>46</v>
       </c>
       <c r="N51" s="6" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="O51" s="6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="P51" s="18" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="Q51" s="6" t="s">
         <v>113</v>
@@ -5431,7 +5431,7 @@
         <v>43</v>
       </c>
       <c r="S51" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T51" s="6"/>
       <c r="U51" s="6"/>
@@ -5449,7 +5449,7 @@
         <v>38</v>
       </c>
       <c r="AC51" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="52" spans="1:29">
@@ -5466,25 +5466,25 @@
         <v>30</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G52" s="6" t="s">
         <v>33</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I52" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J52" s="6" t="s">
         <v>34</v>
       </c>
       <c r="K52" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="L52" s="6" t="s">
         <v>34</v>
@@ -5493,10 +5493,10 @@
         <v>46</v>
       </c>
       <c r="N52" s="6" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="O52" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="P52" s="18" t="s">
         <v>70</v>
@@ -5508,7 +5508,7 @@
         <v>43</v>
       </c>
       <c r="S52" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T52" s="6"/>
       <c r="U52" s="6"/>
@@ -5526,7 +5526,7 @@
         <v>38</v>
       </c>
       <c r="AC52" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="53" spans="1:29">
@@ -5543,25 +5543,25 @@
         <v>30</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G53" s="6" t="s">
         <v>33</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J53" s="6" t="s">
         <v>34</v>
       </c>
       <c r="K53" s="6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="L53" s="6" t="s">
         <v>34</v>
@@ -5570,10 +5570,10 @@
         <v>46</v>
       </c>
       <c r="N53" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="O53" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="P53" s="18" t="s">
         <v>148</v>
@@ -5585,7 +5585,7 @@
         <v>43</v>
       </c>
       <c r="S53" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T53" s="6"/>
       <c r="U53" s="6"/>
@@ -5603,7 +5603,7 @@
         <v>38</v>
       </c>
       <c r="AC53" s="11" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="54" spans="1:29">
@@ -5620,25 +5620,25 @@
         <v>30</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G54" s="6" t="s">
         <v>33</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I54" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J54" s="6" t="s">
         <v>34</v>
       </c>
       <c r="K54" s="6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="L54" s="6" t="s">
         <v>34</v>
@@ -5647,13 +5647,13 @@
         <v>46</v>
       </c>
       <c r="N54" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="O54" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="P54" s="18" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="Q54" s="6" t="s">
         <v>113</v>
@@ -5662,7 +5662,7 @@
         <v>43</v>
       </c>
       <c r="S54" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="T54" s="6"/>
       <c r="U54" s="6"/>
@@ -5680,7 +5680,7 @@
         <v>38</v>
       </c>
       <c r="AC54" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="55" spans="1:29">

</xml_diff>

<commit_message>
terakhir temenan iki wes deal gk ono maneh!
</commit_message>
<xml_diff>
--- a/excel/import penawaran.xlsx
+++ b/excel/import penawaran.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/fa_sai/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B807EE-DED8-2940-AC7E-6DD71CE02DB1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4575F92A-A225-2F4F-8930-38F5FBFD4F30}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" xr2:uid="{B264C883-C65C-404D-AD50-16A2D4E1BD84}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -6106,4 +6108,28 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8B298AF-C7EC-1247-98DA-BD0627F64CBA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE3D254-F5AC-524F-A888-6E404C31675C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>